<commit_message>
Time Improved by eleminating Stop words in Extract Skills Draft of threads have been created
</commit_message>
<xml_diff>
--- a/upload_files/Samir_Humbatov__CV_300620_EN__text.xlsx
+++ b/upload_files/Samir_Humbatov__CV_300620_EN__text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>CV ID</t>
   </si>
@@ -55,25 +55,13 @@
     <t>text.txt</t>
   </si>
   <si>
-    <t>5.670</t>
-  </si>
-  <si>
-    <t>international : 3</t>
-  </si>
-  <si>
-    <t>video : 3</t>
-  </si>
-  <si>
-    <t>collaboration : 6</t>
+    <t>8.333</t>
   </si>
   <si>
     <t>networking : 3</t>
   </si>
   <si>
-    <t>security : 8</t>
-  </si>
-  <si>
-    <t>cloud : 3</t>
+    <t>cloud : 2</t>
   </si>
   <si>
     <t>infrastructure : 1</t>
@@ -82,7 +70,7 @@
     <t>english : 1</t>
   </si>
   <si>
-    <t>cisco : 7</t>
+    <t>cisco : 6</t>
   </si>
   <si>
     <t>cisco ccna : 4</t>
@@ -91,7 +79,7 @@
     <t>ccna : 4</t>
   </si>
   <si>
-    <t>routing : 5</t>
+    <t>routing : 2</t>
   </si>
   <si>
     <t>switching : 2</t>
@@ -100,42 +88,27 @@
     <t>ccnp collaboration : 1</t>
   </si>
   <si>
+    <t>collaboration : 5</t>
+  </si>
+  <si>
     <t>administrator : 3</t>
   </si>
   <si>
-    <t>network : 10</t>
-  </si>
-  <si>
-    <t>systems : 9</t>
-  </si>
-  <si>
-    <t>routers : 1</t>
-  </si>
-  <si>
-    <t>switches : 6</t>
+    <t>network : 8</t>
   </si>
   <si>
     <t>wifi : 1</t>
   </si>
   <si>
-    <t>ap : 1</t>
-  </si>
-  <si>
     <t>monitoring : 4</t>
   </si>
   <si>
     <t>process : 1</t>
   </si>
   <si>
-    <t>snmp : 4</t>
-  </si>
-  <si>
     <t>protocols : 1</t>
   </si>
   <si>
-    <t>zabbix : 2</t>
-  </si>
-  <si>
     <t>management : 4</t>
   </si>
   <si>
@@ -154,16 +127,7 @@
     <t>administration : 2</t>
   </si>
   <si>
-    <t>ip : 7</t>
-  </si>
-  <si>
-    <t>cucm : 3</t>
-  </si>
-  <si>
-    <t>uccx : 4</t>
-  </si>
-  <si>
-    <t>firewalls : 3</t>
+    <t>security : 6</t>
   </si>
   <si>
     <t>disaster recovery : 1</t>
@@ -175,54 +139,24 @@
     <t>trading : 1</t>
   </si>
   <si>
-    <t>access control : 2</t>
-  </si>
-  <si>
-    <t>maintenance : 3</t>
+    <t>access : 1</t>
+  </si>
+  <si>
+    <t>systems : 5</t>
   </si>
   <si>
     <t>hybrid : 1</t>
   </si>
   <si>
-    <t>unity : 4</t>
-  </si>
-  <si>
-    <t>cube : 4</t>
-  </si>
-  <si>
-    <t>core : 2</t>
-  </si>
-  <si>
-    <t>servers : 8</t>
-  </si>
-  <si>
-    <t>azure : 4</t>
-  </si>
-  <si>
-    <t>office 365 : 4</t>
+    <t>servers : 6</t>
+  </si>
+  <si>
+    <t>azure : 5</t>
   </si>
   <si>
     <t>technical support : 6</t>
   </si>
   <si>
-    <t>design : 4</t>
-  </si>
-  <si>
-    <t>manage projects : 1</t>
-  </si>
-  <si>
-    <t>vlan : 5</t>
-  </si>
-  <si>
-    <t>acl : 4</t>
-  </si>
-  <si>
-    <t>nat : 4</t>
-  </si>
-  <si>
-    <t>ipsec : 4</t>
-  </si>
-  <si>
     <t>migration : 6</t>
   </si>
   <si>
@@ -238,25 +172,16 @@
     <t>integration : 2</t>
   </si>
   <si>
-    <t>ivr : 2</t>
-  </si>
-  <si>
     <t>mobility : 1</t>
   </si>
   <si>
     <t>tuning : 2</t>
   </si>
   <si>
-    <t>communication : 1</t>
-  </si>
-  <si>
-    <t>azure cloud : 2</t>
-  </si>
-  <si>
     <t>data center : 1</t>
   </si>
   <si>
-    <t>firewall : 2</t>
+    <t>switches : 5</t>
   </si>
   <si>
     <t>analog : 3</t>
@@ -271,10 +196,7 @@
     <t>engineer : 1</t>
   </si>
   <si>
-    <t>director : 2</t>
-  </si>
-  <si>
-    <t>travel : 1</t>
+    <t>director : 1</t>
   </si>
   <si>
     <t>global : 1</t>
@@ -283,7 +205,7 @@
     <t>planning : 1</t>
   </si>
   <si>
-    <t>asm : 1</t>
+    <t>design : 3</t>
   </si>
   <si>
     <t>hardware : 2</t>
@@ -295,73 +217,7 @@
     <t>research : 1</t>
   </si>
   <si>
-    <t>eigrp : 2</t>
-  </si>
-  <si>
-    <t>ospf : 2</t>
-  </si>
-  <si>
-    <t>vpn : 2</t>
-  </si>
-  <si>
-    <t>frame relay : 2</t>
-  </si>
-  <si>
-    <t>hsrp : 2</t>
-  </si>
-  <si>
-    <t>ssl : 2</t>
-  </si>
-  <si>
-    <t>vtp : 2</t>
-  </si>
-  <si>
-    <t>stp : 2</t>
-  </si>
-  <si>
-    <t>ssh : 2</t>
-  </si>
-  <si>
-    <t>syslog : 2</t>
-  </si>
-  <si>
-    <t>ipv4 : 1</t>
-  </si>
-  <si>
-    <t>ipv6 : 2</t>
-  </si>
-  <si>
-    <t>tcp : 2</t>
-  </si>
-  <si>
-    <t>udp : 2</t>
-  </si>
-  <si>
-    <t>ftp : 2</t>
-  </si>
-  <si>
-    <t>smtp : 2</t>
-  </si>
-  <si>
-    <t>http : 2</t>
-  </si>
-  <si>
-    <t>https : 2</t>
-  </si>
-  <si>
-    <t>sip : 2</t>
-  </si>
-  <si>
-    <t>dhcp : 2</t>
-  </si>
-  <si>
-    <t>dns : 2</t>
-  </si>
-  <si>
-    <t>pbx : 2</t>
-  </si>
-  <si>
-    <t>spark : 2</t>
+    <t>vlan : 3</t>
   </si>
   <si>
     <t>os : 2</t>
@@ -370,31 +226,130 @@
     <t>virtualization : 2</t>
   </si>
   <si>
-    <t>backup : 2</t>
-  </si>
-  <si>
-    <t>ad : 2</t>
-  </si>
-  <si>
-    <t>sql server : 2</t>
+    <t>backup : 1</t>
+  </si>
+  <si>
+    <t>sql : 1</t>
   </si>
   <si>
     <t>microsoft server : 2</t>
   </si>
   <si>
-    <t>windows xp : 1</t>
-  </si>
-  <si>
-    <t>high availability : 1</t>
-  </si>
-  <si>
     <t>installation : 1</t>
   </si>
   <si>
     <t>manager : 1</t>
   </si>
   <si>
-    <t>it : 2</t>
+    <t>snmp : 2</t>
+  </si>
+  <si>
+    <t>zabbix : 1</t>
+  </si>
+  <si>
+    <t>uccx : 2</t>
+  </si>
+  <si>
+    <t>firewalls : 1</t>
+  </si>
+  <si>
+    <t>access control : 1</t>
+  </si>
+  <si>
+    <t>unity : 2</t>
+  </si>
+  <si>
+    <t>cube : 2</t>
+  </si>
+  <si>
+    <t>core : 1</t>
+  </si>
+  <si>
+    <t>acl : 2</t>
+  </si>
+  <si>
+    <t>nat : 2</t>
+  </si>
+  <si>
+    <t>ipsec : 2</t>
+  </si>
+  <si>
+    <t>ivr : 1</t>
+  </si>
+  <si>
+    <t>azure cloud : 1</t>
+  </si>
+  <si>
+    <t>firewall : 1</t>
+  </si>
+  <si>
+    <t>eigrp : 1</t>
+  </si>
+  <si>
+    <t>ospf : 1</t>
+  </si>
+  <si>
+    <t>vpn : 1</t>
+  </si>
+  <si>
+    <t>frame relay : 1</t>
+  </si>
+  <si>
+    <t>hsrp : 1</t>
+  </si>
+  <si>
+    <t>ssl : 1</t>
+  </si>
+  <si>
+    <t>vtp : 1</t>
+  </si>
+  <si>
+    <t>stp : 1</t>
+  </si>
+  <si>
+    <t>ssh : 1</t>
+  </si>
+  <si>
+    <t>syslog : 1</t>
+  </si>
+  <si>
+    <t>ipv6 : 1</t>
+  </si>
+  <si>
+    <t>tcp : 1</t>
+  </si>
+  <si>
+    <t>udp : 1</t>
+  </si>
+  <si>
+    <t>ftp : 1</t>
+  </si>
+  <si>
+    <t>smtp : 1</t>
+  </si>
+  <si>
+    <t>http : 1</t>
+  </si>
+  <si>
+    <t>https : 1</t>
+  </si>
+  <si>
+    <t>sip : 1</t>
+  </si>
+  <si>
+    <t>dhcp : 1</t>
+  </si>
+  <si>
+    <t>dns : 1</t>
+  </si>
+  <si>
+    <t>spark : 1</t>
+  </si>
+  <si>
+    <t>ad : 1</t>
+  </si>
+  <si>
+    <t>sql server : 1</t>
   </si>
   <si>
     <t>it manager : 1</t>
@@ -403,10 +358,7 @@
     <t>analysis : 1</t>
   </si>
   <si>
-    <t>5.555</t>
-  </si>
-  <si>
-    <t>10.0</t>
+    <t>9.090</t>
   </si>
   <si>
     <t>0.0</t>
@@ -750,7 +702,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -818,19 +770,16 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1321,81 +1270,6 @@
     <row r="100" spans="5:5">
       <c r="E100" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="101" spans="5:5">
-      <c r="E101" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="102" spans="5:5">
-      <c r="E102" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="103" spans="5:5">
-      <c r="E103" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="104" spans="5:5">
-      <c r="E104" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="105" spans="5:5">
-      <c r="E105" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="106" spans="5:5">
-      <c r="E106" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="107" spans="5:5">
-      <c r="E107" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="108" spans="5:5">
-      <c r="E108" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="109" spans="5:5">
-      <c r="E109" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="110" spans="5:5">
-      <c r="E110" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="111" spans="5:5">
-      <c r="E111" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="112" spans="5:5">
-      <c r="E112" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="113" spans="5:5">
-      <c r="E113" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="114" spans="5:5">
-      <c r="E114" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="115" spans="5:5">
-      <c r="E115" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>